<commit_message>
Static text at top + panel bids
The text at the top of the bid can now change with the bid.
The panel bids form (a variant of class bid) has been added.
</commit_message>
<xml_diff>
--- a/To Do List for new Site.xlsx
+++ b/To Do List for new Site.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="25560" windowHeight="15920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="103">
   <si>
     <t>Thing to do</t>
   </si>
@@ -132,9 +132,6 @@
     <t>View User Ticket Status</t>
   </si>
   <si>
-    <t>View User Bids</t>
-  </si>
-  <si>
     <t>View User Schedule</t>
   </si>
   <si>
@@ -243,15 +240,9 @@
     <t>Calendar for - show &amp; special, conference, volunteer</t>
   </si>
   <si>
-    <t xml:space="preserve">Connection highly editable static content </t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
-    <t>Beth</t>
-  </si>
-  <si>
     <t>Login Check on any Editing by regular user</t>
   </si>
   <si>
@@ -268,6 +259,75 @@
   </si>
   <si>
     <t>Set Act Tech Info &amp; Pick Rehearsal</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>1/2 Done</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>trivial, done</t>
+  </si>
+  <si>
+    <t>Betty</t>
+  </si>
+  <si>
+    <t>Connection highly editable static content in a page</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>These are permutations of the same thing, so fairly cut/copy/paste-able</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>assigned</t>
+  </si>
+  <si>
+    <t>unassigned</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Very similar</t>
+  </si>
+  <si>
+    <t>includes change to page for ad display</t>
+  </si>
+  <si>
+    <t>very similar, and simpler than 24/25</t>
+  </si>
+  <si>
+    <t>View User Bids by User</t>
+  </si>
+  <si>
+    <t>Betty*</t>
+  </si>
+  <si>
+    <t>preferably as a popover or drop down from sidebar</t>
+  </si>
+  <si>
+    <t>needs to link to Jon's fixes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">order\ </t>
+  </si>
+  <si>
+    <t>3/4 Done</t>
   </si>
 </sst>
 </file>
@@ -313,12 +373,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -330,7 +396,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -338,8 +404,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -347,14 +421,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -684,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -697,9 +796,10 @@
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="20">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -718,13 +818,19 @@
       <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1">
+      <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="3" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1">
+    <row r="3" spans="1:12" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -738,10 +844,13 @@
         <v>11</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1">
+        <v>85</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="31" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -760,8 +869,18 @@
       <c r="F4" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1">
+      <c r="H4" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="3">
+        <f>COUNTIF(F:F,J4)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -777,8 +896,21 @@
       <c r="F5" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1">
+      <c r="G5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="3">
+        <f>COUNTIF(F:F,J5)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
@@ -794,8 +926,15 @@
       <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1">
+      <c r="J6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="3">
+        <f>COUNTIF(F:F,J6)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -808,22 +947,50 @@
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1">
+      <c r="F7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" s="3">
+        <f>COUNTIF(F:F,J7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="3" customFormat="1">
+      <c r="F8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -836,27 +1003,60 @@
       <c r="E9" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1">
-      <c r="A10" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <f>COUNTIF(D:D,I9)</f>
+        <v>21</v>
+      </c>
+      <c r="K9" s="3">
+        <f>COUNTIFS(D:D,I9,F:F,"*")</f>
+        <v>18</v>
+      </c>
+      <c r="L9" s="3">
+        <f>J9-K9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="9" customFormat="1">
+      <c r="A10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1">
+      <c r="I10" s="13">
+        <v>2</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" ref="J10:J12" si="0">COUNTIF(D:D,I10)</f>
+        <v>25</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" ref="K10:K12" si="1">COUNTIFS(D:D,I10,F:F,"*")</f>
+        <v>7</v>
+      </c>
+      <c r="L10" s="9">
+        <f t="shared" ref="L10:L12" si="2">J10-K10</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -867,14 +1067,48 @@
       <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1"/>
-    <row r="13" spans="1:6">
+      <c r="F11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="2">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1">
+      <c r="I12" s="2">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -887,8 +1121,17 @@
       <c r="E14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="F14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -901,8 +1144,15 @@
       <c r="E15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -915,8 +1165,15 @@
       <c r="E16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -929,8 +1186,15 @@
       <c r="E17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -943,8 +1207,12 @@
       <c r="E18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -957,8 +1225,12 @@
       <c r="E19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -971,10 +1243,14 @@
       <c r="E20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -985,8 +1261,12 @@
       <c r="E21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1003,39 +1283,46 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
         <v>45</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>46</v>
-      </c>
       <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
@@ -1044,10 +1331,13 @@
       <c r="E26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="H26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1058,10 +1348,13 @@
       <c r="E27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="H27" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1072,10 +1365,11 @@
       <c r="E28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1087,12 +1381,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -1106,10 +1400,10 @@
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1123,12 +1417,12 @@
         <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1140,10 +1434,10 @@
         <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -1157,47 +1451,47 @@
         <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
         <v>40</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
         <v>41</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="F38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" t="s">
+      <c r="B39" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="D39">
         <v>1</v>
       </c>
@@ -1205,18 +1499,18 @@
         <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:7">
       <c r="A41" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="3" customFormat="1">
+    <row r="42" spans="1:7" s="3" customFormat="1">
       <c r="A42" s="3" t="s">
         <v>26</v>
       </c>
@@ -1232,8 +1526,11 @@
       <c r="F42" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -1250,21 +1547,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
+    <row r="44" spans="1:7" s="10" customFormat="1">
+      <c r="A44" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="D44" s="3">
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="B44" s="10">
+        <v>1</v>
+      </c>
+      <c r="D44" s="11">
+        <v>1</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -1278,24 +1578,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46" t="s">
+    <row r="46" spans="1:7" s="8" customFormat="1">
+      <c r="A46" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="8">
+        <v>1</v>
+      </c>
+      <c r="D46" s="9">
+        <v>1</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
         <v>37</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="D46" s="3">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>38</v>
-      </c>
       <c r="B47">
         <v>1</v>
       </c>
@@ -1306,9 +1606,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1322,7 +1622,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1341,7 +1641,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -1350,12 +1650,12 @@
         <v>2</v>
       </c>
       <c r="E52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1364,12 +1664,12 @@
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -1378,12 +1678,12 @@
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -1392,12 +1692,12 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1411,7 +1711,7 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -1420,12 +1720,12 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -1434,12 +1734,12 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1448,12 +1748,12 @@
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -1465,23 +1765,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
-      <c r="A62" t="s">
-        <v>71</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62" t="s">
+    <row r="62" spans="1:5" s="8" customFormat="1">
+      <c r="A62" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="8">
+        <v>1</v>
+      </c>
+      <c r="D62" s="8">
+        <v>1</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -1495,7 +1795,7 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1507,9 +1807,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -1521,9 +1821,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -1535,14 +1835,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:7">
       <c r="A68" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
-        <v>62</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1554,9 +1854,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -1568,9 +1868,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -1582,9 +1882,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -1596,9 +1896,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -1610,9 +1910,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -1621,26 +1921,39 @@
         <v>4</v>
       </c>
       <c r="E74" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
-      <c r="A77" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:7">
       <c r="D79">
         <f>COUNTIF(D2:D78,"&gt;0")</f>
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="F79">
+        <f>COUNTIF(F2:F78,"*")</f>
+        <v>26</v>
+      </c>
+      <c r="G79">
+        <f>D79-F79</f>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H14:H21"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="H27:H28"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>